<commit_message>
testcases to the new sprint items added
</commit_message>
<xml_diff>
--- a/doc/projectFiles/Testcases.xlsx
+++ b/doc/projectFiles/Testcases.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestTemplate-Req1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestTemplate-Req2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestTemplate-Req3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestTemplate-Req4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="121">
   <si>
     <t>Tests zu Requiremets 1 - Veranstaltungsverwaltung</t>
   </si>
@@ -188,6 +191,195 @@
   </si>
   <si>
     <t>Testcase number</t>
+  </si>
+  <si>
+    <t>Tests zu Requiremets 3 - Tweet-Filterung</t>
+  </si>
+  <si>
+    <t>3-2: Für die gesammelten Tweets einer Veranstaltung können bereits angelegte Filteransichten geladen, editiert und wieder gespeichert werden.</t>
+  </si>
+  <si>
+    <t>3-1: Für die gesammelten Tweets einer Veranstaltung können Filteransichten (basierenden auf Schlagwörter-Matching oder Datum) angelegt und gespeichert werden.</t>
+  </si>
+  <si>
+    <t>3-3: Einzelne Tweets einer Veranstaltung können für eine bestehende Filteransicht manuell ausgeblendet werden.</t>
+  </si>
+  <si>
+    <t>3-4: Einzelne Tweets einer Veranstaltung können für diese Veranstaltung manuell gelöscht werden.</t>
+  </si>
+  <si>
+    <t>2-1: Für die Stimmungs-Analyse kann die vorgefertigte Stimmungs-Liste verwendet werden. In dieser werden Keywords mit entsprechender Gewichtung gespeichert. Durch diese Keywords kann zu jedem Tweet eine positive oder negative Stimmung zugeordnet werden.</t>
+  </si>
+  <si>
+    <t>2-2: Für die Stimmungs-Analyse können zur Stimmungs-Liste eigene Keywords mit Gewichtung hinzugefügt werden, um damit eine neue Liste von Stimmungswörtern zu erzeugen, welche in allen Analysen verwendet werden kann.</t>
+  </si>
+  <si>
+    <t>2-3: Für einen bestimmten Tweet-Filter kann eine Stimmungs-Analyse mit einer vorhandenen Stimmungsliste durchgeführt und gespeichert werden.</t>
+  </si>
+  <si>
+    <t>2-4: Die Analyse-Resultate von durchgeführten Analysen können graphisch angezeigt werden.</t>
+  </si>
+  <si>
+    <t>Tests zu Requiremets 2 - Tweet-Analyse</t>
+  </si>
+  <si>
+    <t>Tests zu Requiremets 4 - Export</t>
+  </si>
+  <si>
+    <t>4-1: Die gesammelten Tweets können pro Veranstaltung im .csv Format exportiert werden.</t>
+  </si>
+  <si>
+    <t>4-2: Resultate der Stimmungsanalyse können pro Veranstaltung exportiert werden, im .csv Format.</t>
+  </si>
+  <si>
+    <t>Create a filter</t>
+  </si>
+  <si>
+    <t>View of tweets in the tweets table</t>
+  </si>
+  <si>
+    <t>From navigation bar on left side, one can navigate to the table of all tweets</t>
+  </si>
+  <si>
+    <t>This view includes: the tweets table, a dropdown list of the events, of the filter for each event,</t>
+  </si>
+  <si>
+    <t>filter- and analysis buttons, and a tweet text search field</t>
+  </si>
+  <si>
+    <t>When an event is selected, a filter can be created with the "Create Filter" button.</t>
+  </si>
+  <si>
+    <t>Choosing of an event</t>
+  </si>
+  <si>
+    <t>In the dropdown list of events, one of the events previously created can be chosen by their names.</t>
+  </si>
+  <si>
+    <t>Filter creation and applying is only possible if one valid event is selected.</t>
+  </si>
+  <si>
+    <t>One entry "all" also exists, showing all tweets in the system.</t>
+  </si>
+  <si>
+    <t>Only choosing an event and no filter shows all tweets of that event.</t>
+  </si>
+  <si>
+    <t>Choosing of a filter</t>
+  </si>
+  <si>
+    <t>The filter is applied to the Tweets table after selection.</t>
+  </si>
+  <si>
+    <t>Creation - Text</t>
+  </si>
+  <si>
+    <t>Empty text shall also be possible.</t>
+  </si>
+  <si>
+    <t>Text shall be saved and displayed as they are entered (e.g. right case and right letters).</t>
+  </si>
+  <si>
+    <t>All special characters and combinations of the german keyboard shall be valid, and shall be matched right in the tweets.</t>
+  </si>
+  <si>
+    <t>Creation - Date From / To</t>
+  </si>
+  <si>
+    <t>Only tweets in the given timeframe shall be visible with the created filter.</t>
+  </si>
+  <si>
+    <t>Creation - User</t>
+  </si>
+  <si>
+    <t>Empty date or one missing date is also permitted.</t>
+  </si>
+  <si>
+    <t>Creation - Location</t>
+  </si>
+  <si>
+    <t>Editing a filter</t>
+  </si>
+  <si>
+    <t>A previously created filter for an event can be selected and therefore applied again.</t>
+  </si>
+  <si>
+    <t>The filter criteria are applied in the right way.</t>
+  </si>
+  <si>
+    <t>The filter criteria can be edited and can again be saved and applied.</t>
+  </si>
+  <si>
+    <t>In the dropdown list of filters, one of the filter that was previously created for the selected event can be chosen by ist name.</t>
+  </si>
+  <si>
+    <t>There is also a no-filter blank option, that displays all tweets for the event.</t>
+  </si>
+  <si>
+    <t>Editing - Text</t>
+  </si>
+  <si>
+    <t>Editing - Date From / To</t>
+  </si>
+  <si>
+    <t>Editing - User</t>
+  </si>
+  <si>
+    <t>Editing - Location</t>
+  </si>
+  <si>
+    <t>Creation of a filter - Cancel</t>
+  </si>
+  <si>
+    <t>While creating a filter and adding criteria and then hitting cancel, the filter shall not be added to the event.</t>
+  </si>
+  <si>
+    <t>No filter shall be saved or applied.</t>
+  </si>
+  <si>
+    <t>Tweet text search</t>
+  </si>
+  <si>
+    <t>Through the text search field, the tweets can be filtered by a given text.</t>
+  </si>
+  <si>
+    <t>Only tweets matching the given text shall be visible.</t>
+  </si>
+  <si>
+    <t>Paging</t>
+  </si>
+  <si>
+    <t>Only a selected amount of tweets is shown on each page, if the result is too great for one page.</t>
+  </si>
+  <si>
+    <t>Still, the filters are working in the right way (that filters all tweets, not only on some pages).</t>
+  </si>
+  <si>
+    <t>Starting an analysis</t>
+  </si>
+  <si>
+    <t>An analysis can be started for a selected filter for the tweets of an event.</t>
+  </si>
+  <si>
+    <t>Editing of a filter - Cancel</t>
+  </si>
+  <si>
+    <t>While editing a filter and editing criteria and then hitting cancel, the filter shall not be updated.</t>
+  </si>
+  <si>
+    <t>The filter shall not be edited, no new criteria shall be applied.</t>
+  </si>
+  <si>
+    <t>Filter from other events do not apply to a new chosen event.</t>
+  </si>
+  <si>
+    <t>Multi-linguality</t>
+  </si>
+  <si>
+    <t>The creation dialogues of filter, and the tweets table view changes according to the selected languages.</t>
+  </si>
+  <si>
+    <t>After filling in the filter properties, the filter is created and assigned to the event.</t>
   </si>
 </sst>
 </file>
@@ -530,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="G116" sqref="G116"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1164,4 +1356,702 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="1"/>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:E119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1"/>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1"/>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1"/>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="D15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="D27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="D40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="D41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="D44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="D48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="D52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="D57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="D58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="D59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="D60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="D61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="D64" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="D65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="D66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="D69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="D70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="D71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="D72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="D73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="D74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76">
+        <v>11</v>
+      </c>
+      <c r="C76" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="D77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="D78" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="D79" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="D80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="D82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="D83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="D84" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86">
+        <v>12</v>
+      </c>
+      <c r="C86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="D87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="D88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="D90" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="D91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="D92" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="D95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="D96" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="D97" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="D98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="D99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="D100" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102">
+        <v>14</v>
+      </c>
+      <c r="C102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="D103" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="D104" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106">
+        <v>15</v>
+      </c>
+      <c r="C106" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="D107" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="D108" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110">
+        <v>16</v>
+      </c>
+      <c r="C110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="D111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="D112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114">
+        <v>17</v>
+      </c>
+      <c r="C114" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4">
+      <c r="D115" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4">
+      <c r="D116" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="B118">
+        <v>18</v>
+      </c>
+      <c r="C118" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4">
+      <c r="D119" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test cases updated (typos and structure fixed) user docu updated to new sprint content manual test report for this sprint defects from manual test added to defects table
</commit_message>
<xml_diff>
--- a/doc/projectFiles/Testcases.xlsx
+++ b/doc/projectFiles/Testcases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
   <si>
     <t>Tests zu Requiremets 1 - Veranstaltungsverwaltung</t>
   </si>
@@ -322,9 +322,6 @@
     <t>Editing - Date From / To</t>
   </si>
   <si>
-    <t>Editing - User</t>
-  </si>
-  <si>
     <t>Editing - Location</t>
   </si>
   <si>
@@ -380,6 +377,12 @@
   </si>
   <si>
     <t>After filling in the filter properties, the filter is created and assigned to the event.</t>
+  </si>
+  <si>
+    <t>When applying the filter, the right tweets shall be shown.</t>
+  </si>
+  <si>
+    <t>Editing - Language</t>
   </si>
 </sst>
 </file>
@@ -1412,13 +1415,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="1"/>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1434,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E119"/>
+  <dimension ref="B1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1529,7 +1532,7 @@
     </row>
     <row r="15" spans="2:5">
       <c r="D15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -1547,7 +1550,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="D19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -1811,213 +1814,233 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="2:4">
-      <c r="B76">
+    <row r="75" spans="2:4">
+      <c r="D75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77">
         <v>11</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
-      <c r="D77" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="D78" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="D79" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="D80" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="D81" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="D82" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="D83" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="D84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="D85" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="86" spans="2:4">
-      <c r="B86">
+      <c r="D86" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88">
         <v>12</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4">
-      <c r="D87" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4">
-      <c r="D88" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="D89" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="D90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="D91" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="D92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="D93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="D94" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4">
-      <c r="B94">
-        <v>13</v>
-      </c>
-      <c r="C94" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="D95" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4">
-      <c r="D96" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="2:4">
-      <c r="D97" t="s">
-        <v>86</v>
+      <c r="B97">
+        <v>13</v>
+      </c>
+      <c r="C97" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="2:4">
       <c r="D98" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="D99" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="D100" t="s">
-        <v>32</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="D101" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="2:4">
-      <c r="B102">
-        <v>14</v>
-      </c>
-      <c r="C102" t="s">
-        <v>103</v>
+      <c r="D102" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="D103" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="D104" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="2:4">
       <c r="B106">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C106" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="2:4">
       <c r="D107" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="D108" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C110" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="2:4">
       <c r="D111" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="D112" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="2:4">
       <c r="B114">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C114" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="D115" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="D116" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="2:4">
       <c r="B118">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C118" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="2:4">
       <c r="D119" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4">
+      <c r="D120" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4">
+      <c r="B122">
+        <v>18</v>
+      </c>
+      <c r="C122" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4">
+      <c r="D123" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
language texts updated. testcases and user documentation updated. manual test report added. defect table updated according to findings of test.
</commit_message>
<xml_diff>
--- a/doc/projectFiles/Testcases.xlsx
+++ b/doc/projectFiles/Testcases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
   <si>
     <t>Tests zu Requiremets 1 - Veranstaltungsverwaltung</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Only tweets in the given timeframe shall be visible with the created filter.</t>
   </si>
   <si>
-    <t>Creation - User</t>
-  </si>
-  <si>
     <t>Empty date or one missing date is also permitted.</t>
   </si>
   <si>
@@ -383,6 +380,180 @@
   </si>
   <si>
     <t>Editing - Language</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - delete word</t>
+  </si>
+  <si>
+    <t>The selected word is deleted.</t>
+  </si>
+  <si>
+    <t>After confirmation, the word cannot be found anymore.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - edit word + cancel</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - delete word + cancel</t>
+  </si>
+  <si>
+    <t>The edit form for the selected word is invoked.</t>
+  </si>
+  <si>
+    <t>After cancelling deletion, the word is not deleted.</t>
+  </si>
+  <si>
+    <t>After editing values, the editing is canceled. No properties for the word is updated.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - add word</t>
+  </si>
+  <si>
+    <t>A new word can be configured.</t>
+  </si>
+  <si>
+    <t>After saving, the word is added to the list.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - add word: Language</t>
+  </si>
+  <si>
+    <t>When adding a new word, the language property can be selected from a list.</t>
+  </si>
+  <si>
+    <t>List is filled with languages already configured on the db.</t>
+  </si>
+  <si>
+    <t>The selected language is properly saved.</t>
+  </si>
+  <si>
+    <t>All configured languages can be selected.</t>
+  </si>
+  <si>
+    <t>Language is a mandatory field.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenace - add word + cancel</t>
+  </si>
+  <si>
+    <t>A new word is created, the the creation is cancelled.</t>
+  </si>
+  <si>
+    <t>The word is not added to the list or to the db.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - add word: Word</t>
+  </si>
+  <si>
+    <t>When adding a new word, this word can only be stored in the char-set of the database.</t>
+  </si>
+  <si>
+    <t>Word is a mandatory field.</t>
+  </si>
+  <si>
+    <t>Within this char-set, all available characters can be saved correctly, and retrieved correctly.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - add word: Weight</t>
+  </si>
+  <si>
+    <t>When adding a new word, the weight of this word can be selected with a spinner field.</t>
+  </si>
+  <si>
+    <t>The spinner field only gives values between -5 and +5.</t>
+  </si>
+  <si>
+    <t>The values are saved correctly and retrieved correctly.</t>
+  </si>
+  <si>
+    <t>Weight is a mandatory field.</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - edit word: Language</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - edit word: Word</t>
+  </si>
+  <si>
+    <t>Sentiment maintenance - edit word: Weight</t>
+  </si>
+  <si>
+    <t>When editing a word, the language property can be selected from a list.</t>
+  </si>
+  <si>
+    <t>When editing a word, this word can only be stored in the char-set of the database.</t>
+  </si>
+  <si>
+    <t>When editing a word, the weight of this word can be selected with a spinner field.</t>
+  </si>
+  <si>
+    <t>Delete filter</t>
+  </si>
+  <si>
+    <t>A filter can be deleted with the "delete filter" button.</t>
+  </si>
+  <si>
+    <t>After deletion, the filter cannot be found anymore.</t>
+  </si>
+  <si>
+    <t>Delete filter - cancel</t>
+  </si>
+  <si>
+    <t>When cancelling the deletion of a filter, it is not deleted and can still be found.</t>
+  </si>
+  <si>
+    <t>Tweet deletion</t>
+  </si>
+  <si>
+    <t>Selected tweets can be deleted with the "delete Tweets" button.</t>
+  </si>
+  <si>
+    <t>The do not come into the system for this event again, after deleting.</t>
+  </si>
+  <si>
+    <t>Deletion affects all filters for the selected event.</t>
+  </si>
+  <si>
+    <t>"check all" checkbox works correctly.</t>
+  </si>
+  <si>
+    <t>Tweet deletion - cancel</t>
+  </si>
+  <si>
+    <t>When cancelling the deletion of the selected tweets, they are not deleted.</t>
+  </si>
+  <si>
+    <t>Tweet ignoring</t>
+  </si>
+  <si>
+    <t>Single tweets can be ignored in the current selected filter with the "ignore" button.</t>
+  </si>
+  <si>
+    <t>This ignore status is correctly saved for the filter.</t>
+  </si>
+  <si>
+    <t>The ignored tweets are not considered in an analysis.</t>
+  </si>
+  <si>
+    <t>The ignore status can be toggled on / off by the user.</t>
+  </si>
+  <si>
+    <t>Searching for events</t>
+  </si>
+  <si>
+    <t>With the text search field, the showed events can be searched</t>
+  </si>
+  <si>
+    <t>Creation - Language</t>
+  </si>
+  <si>
+    <t>One of the languages configured on the database can be selected.</t>
+  </si>
+  <si>
+    <t>All of them are possible for selection.</t>
+  </si>
+  <si>
+    <t>None can be selected.</t>
   </si>
 </sst>
 </file>
@@ -723,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38:D43"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119:D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1355,6 +1526,19 @@
         <v>54</v>
       </c>
     </row>
+    <row r="119" spans="2:4">
+      <c r="B119">
+        <v>18</v>
+      </c>
+      <c r="C119" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4">
+      <c r="D120" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1363,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:D78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1415,13 +1599,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="1"/>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1429,6 +1613,264 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="1"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="D25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="D29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="D30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="D33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="D34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="D37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="D41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="D42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="D45" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="D46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="D47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="D48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="D49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="D52" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="D53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="D54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56">
+        <v>26</v>
+      </c>
+      <c r="C56" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="D57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="D58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="D59" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="D60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="D63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="D64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="D65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="D66" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="D67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69">
+        <v>25</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="D70" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="D71" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="D72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74">
+        <v>26</v>
+      </c>
+      <c r="C74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="D75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="D76" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="D77" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="D78" t="s">
+        <v>149</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1437,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E123"/>
+  <dimension ref="B1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1532,7 +1974,7 @@
     </row>
     <row r="15" spans="2:5">
       <c r="D15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -1550,7 +1992,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="D19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -1578,7 +2020,7 @@
     </row>
     <row r="25" spans="2:4">
       <c r="D25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -1588,7 +2030,7 @@
     </row>
     <row r="27" spans="2:4">
       <c r="D27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -1669,7 +2111,7 @@
     </row>
     <row r="44" spans="2:4">
       <c r="D44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -1682,7 +2124,7 @@
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -1720,327 +2162,412 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="D56" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="D58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4">
-      <c r="D59" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="2:4">
-      <c r="D60" t="s">
-        <v>39</v>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="D61" t="s">
-        <v>32</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="D62" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="2:4">
-      <c r="B63">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4">
-      <c r="D64" t="s">
-        <v>94</v>
+      <c r="D63" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="D65" t="s">
-        <v>95</v>
+      <c r="B65">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="D66" t="s">
-        <v>96</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="D67" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="2:4">
-      <c r="B68">
-        <v>10</v>
-      </c>
-      <c r="C68" t="s">
-        <v>99</v>
+      <c r="D68" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="D69" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="D70" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="D71" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="D72" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4">
-      <c r="D73" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="2:4">
-      <c r="D74" t="s">
-        <v>32</v>
+      <c r="B74">
+        <v>11</v>
+      </c>
+      <c r="C74" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="D75" t="s">
-        <v>120</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="D76" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="2:4">
-      <c r="B77">
-        <v>11</v>
-      </c>
-      <c r="C77" t="s">
-        <v>100</v>
+      <c r="D77" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="D78" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="D79" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="D80" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="D81" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="D82" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="D83" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4">
-      <c r="D84" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="D85" t="s">
-        <v>89</v>
+      <c r="B85">
+        <v>12</v>
+      </c>
+      <c r="C85" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="D86" t="s">
-        <v>120</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="D87" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:4">
-      <c r="B88">
-        <v>12</v>
-      </c>
-      <c r="C88" t="s">
-        <v>101</v>
+      <c r="D88" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="D89" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="D90" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="D91" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="D92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4">
-      <c r="D93" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="D94" t="s">
-        <v>32</v>
+      <c r="B94">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="D95" t="s">
-        <v>120</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="D96" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="2:4">
-      <c r="B97">
-        <v>13</v>
-      </c>
-      <c r="C97" t="s">
-        <v>121</v>
+      <c r="D97" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="2:4">
       <c r="D98" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="D99" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="D100" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="D101" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4">
-      <c r="D102" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="2:4">
-      <c r="D103" t="s">
-        <v>32</v>
+      <c r="B103">
+        <v>14</v>
+      </c>
+      <c r="C103" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="D104" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4">
-      <c r="B106">
-        <v>14</v>
-      </c>
-      <c r="C106" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="105" spans="2:4">
+      <c r="D105" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="107" spans="2:4">
-      <c r="D107" t="s">
-        <v>103</v>
+      <c r="B107">
+        <v>15</v>
+      </c>
+      <c r="C107" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="D108" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4">
-      <c r="B110">
-        <v>15</v>
-      </c>
-      <c r="C110" t="s">
         <v>105</v>
       </c>
     </row>
+    <row r="109" spans="2:4">
+      <c r="D109" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="111" spans="2:4">
-      <c r="D111" t="s">
-        <v>106</v>
+      <c r="B111">
+        <v>16</v>
+      </c>
+      <c r="C111" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="D112" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4">
-      <c r="B114">
-        <v>16</v>
-      </c>
-      <c r="C114" t="s">
         <v>108</v>
       </c>
     </row>
+    <row r="113" spans="2:4">
+      <c r="D113" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="115" spans="2:4">
-      <c r="D115" t="s">
-        <v>109</v>
+      <c r="B115">
+        <v>17</v>
+      </c>
+      <c r="C115" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="D116" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4">
-      <c r="B118">
-        <v>17</v>
-      </c>
-      <c r="C118" t="s">
         <v>113</v>
       </c>
     </row>
+    <row r="117" spans="2:4">
+      <c r="D117" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="119" spans="2:4">
-      <c r="D119" t="s">
-        <v>114</v>
+      <c r="B119">
+        <v>18</v>
+      </c>
+      <c r="C119" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="D120" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="2:4">
       <c r="B122">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C122" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
     </row>
     <row r="123" spans="2:4">
       <c r="D123" t="s">
-        <v>118</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4">
+      <c r="D124" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4">
+      <c r="B126">
+        <v>20</v>
+      </c>
+      <c r="C126" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4">
+      <c r="D127" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4">
+      <c r="B129">
+        <v>21</v>
+      </c>
+      <c r="C129" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4">
+      <c r="D130" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4">
+      <c r="D131" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4">
+      <c r="D132" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4">
+      <c r="D133" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4">
+      <c r="B135">
+        <v>22</v>
+      </c>
+      <c r="C135" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4">
+      <c r="D136" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4">
+      <c r="B138">
+        <v>23</v>
+      </c>
+      <c r="C138" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4">
+      <c r="D139" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4">
+      <c r="D140" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4">
+      <c r="D141" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4">
+      <c r="D142" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testcases made camera-ready install-instructions updated
</commit_message>
<xml_diff>
--- a/doc/projectFiles/Testcases.xlsx
+++ b/doc/projectFiles/Testcases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestTemplate-Req1" sheetId="1" r:id="rId1"/>
@@ -17,25 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
-  <si>
-    <t>Tests zu Requiremets 1 - Veranstaltungsverwaltung</t>
-  </si>
-  <si>
-    <t>1-1: Veranstaltungen können angelegt und gespeichert werden.</t>
-  </si>
-  <si>
-    <t>1-2: Bestehende Veranstaltungen können editiert werden, und die Änderungen können gespeichert werden.</t>
-  </si>
-  <si>
-    <t>1-3: Die Detailansicht zu bestehenden Veranstaltungen kann aufgerufen werden. In der Detailansicht können weiterführende Funktionen der Veranstaltung aufgerufen werden (Analyse, Tweet-Filter, Export)</t>
-  </si>
-  <si>
-    <t>1-4: Bestehende Veranstaltungen können in einer Tabelle angezeigt werden.</t>
-  </si>
-  <si>
-    <t>1-5: Zu einer bestehenden Veranstaltung werden Tweets für den angegebenen Zeitraum gesammelt.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="192">
   <si>
     <t>Test</t>
   </si>
@@ -193,45 +175,9 @@
     <t>Testcase number</t>
   </si>
   <si>
-    <t>Tests zu Requiremets 3 - Tweet-Filterung</t>
-  </si>
-  <si>
-    <t>3-2: Für die gesammelten Tweets einer Veranstaltung können bereits angelegte Filteransichten geladen, editiert und wieder gespeichert werden.</t>
-  </si>
-  <si>
-    <t>3-1: Für die gesammelten Tweets einer Veranstaltung können Filteransichten (basierenden auf Schlagwörter-Matching oder Datum) angelegt und gespeichert werden.</t>
-  </si>
-  <si>
-    <t>3-3: Einzelne Tweets einer Veranstaltung können für eine bestehende Filteransicht manuell ausgeblendet werden.</t>
-  </si>
-  <si>
-    <t>3-4: Einzelne Tweets einer Veranstaltung können für diese Veranstaltung manuell gelöscht werden.</t>
-  </si>
-  <si>
-    <t>2-1: Für die Stimmungs-Analyse kann die vorgefertigte Stimmungs-Liste verwendet werden. In dieser werden Keywords mit entsprechender Gewichtung gespeichert. Durch diese Keywords kann zu jedem Tweet eine positive oder negative Stimmung zugeordnet werden.</t>
-  </si>
-  <si>
-    <t>2-2: Für die Stimmungs-Analyse können zur Stimmungs-Liste eigene Keywords mit Gewichtung hinzugefügt werden, um damit eine neue Liste von Stimmungswörtern zu erzeugen, welche in allen Analysen verwendet werden kann.</t>
-  </si>
-  <si>
-    <t>2-3: Für einen bestimmten Tweet-Filter kann eine Stimmungs-Analyse mit einer vorhandenen Stimmungsliste durchgeführt und gespeichert werden.</t>
-  </si>
-  <si>
-    <t>2-4: Die Analyse-Resultate von durchgeführten Analysen können graphisch angezeigt werden.</t>
-  </si>
-  <si>
-    <t>Tests zu Requiremets 2 - Tweet-Analyse</t>
-  </si>
-  <si>
     <t>Tests zu Requiremets 4 - Export</t>
   </si>
   <si>
-    <t>4-1: Die gesammelten Tweets können pro Veranstaltung im .csv Format exportiert werden.</t>
-  </si>
-  <si>
-    <t>4-2: Resultate der Stimmungsanalyse können pro Veranstaltung exportiert werden, im .csv Format.</t>
-  </si>
-  <si>
     <t>Create a filter</t>
   </si>
   <si>
@@ -554,6 +500,99 @@
   </si>
   <si>
     <t>None can be selected.</t>
+  </si>
+  <si>
+    <t>Export Button</t>
+  </si>
+  <si>
+    <t>The export button can be found on the right site of the statistics tab.</t>
+  </si>
+  <si>
+    <t>Export of an analysis</t>
+  </si>
+  <si>
+    <t>The export button can only be selected when data is shown in the statistics tab.</t>
+  </si>
+  <si>
+    <t>On click, the shown data can be saved to disk in the .csv format.</t>
+  </si>
+  <si>
+    <t>Export data</t>
+  </si>
+  <si>
+    <t>Only data from the currently selected fiter and analysis is exported.</t>
+  </si>
+  <si>
+    <t>The data is exported in a valid .csv format.</t>
+  </si>
+  <si>
+    <t>Tests zu Requiremets 3 - Tweet-Filter</t>
+  </si>
+  <si>
+    <t>Tests zu Requiremets 2 - Tweet-Analysis</t>
+  </si>
+  <si>
+    <t>Tests zu Requiremets 1 - Event management</t>
+  </si>
+  <si>
+    <t>The data that is exported matches the data of the selected analysis.</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>A .csv file with sentiment word definitions can be imported to the application.</t>
+  </si>
+  <si>
+    <t>The sentiment words with their languages and weightings are correctly stored in the database.</t>
+  </si>
+  <si>
+    <t>Incorrect weighting beyond +5/-5 is not saved.</t>
+  </si>
+  <si>
+    <t>Viewing an analysis</t>
+  </si>
+  <si>
+    <t>For a configured event and a filter, an analysis that was already made</t>
+  </si>
+  <si>
+    <t>and saved to the database can be selected in the statistics view.</t>
+  </si>
+  <si>
+    <t>The report of the analysis results are shown.</t>
+  </si>
+  <si>
+    <t>Analysis results - distribution</t>
+  </si>
+  <si>
+    <t>A table of sentiment distributions is shown for the selected analysis.</t>
+  </si>
+  <si>
+    <t>The shown distribution of sentiments of the analyzed tweets is correct with regards to the assigned sentiment values.</t>
+  </si>
+  <si>
+    <t>The sentiment distriubtions are shown in various charts / diagrams.</t>
+  </si>
+  <si>
+    <t>Analysis results - Charts / Diagrams</t>
+  </si>
+  <si>
+    <t>The distribution is shown in different charts.</t>
+  </si>
+  <si>
+    <t>The chart distributions correspond to the correct distribution of assigned sentiment values.</t>
+  </si>
+  <si>
+    <t>Analysis results - Map</t>
+  </si>
+  <si>
+    <t>and saved to the database can be selected in the maps view.</t>
+  </si>
+  <si>
+    <t>The distribution of the tweets according to their geo-location is shown.</t>
+  </si>
+  <si>
+    <t>The tweets are colored according to their assigned sentiment values.</t>
   </si>
 </sst>
 </file>
@@ -894,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119:D120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -909,562 +948,560 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="1"/>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
+    <row r="6" spans="1:4">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="8" spans="1:4">
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
+      <c r="A8" t="s">
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
+      <c r="D9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="1"/>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" s="1"/>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
+      <c r="D12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="D16" t="s">
-        <v>30</v>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:4">
+      <c r="B17" s="1"/>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:4">
+      <c r="B18" s="1"/>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:4">
+      <c r="B19" s="1"/>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="D20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="1">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
+      <c r="B21" s="1"/>
+      <c r="D21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="1"/>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="1"/>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="1"/>
-      <c r="D24" t="s">
-        <v>34</v>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="1"/>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="1"/>
-      <c r="D26" t="s">
-        <v>39</v>
+      <c r="D26" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="1"/>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="1">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>17</v>
+      <c r="B29" s="1"/>
+      <c r="D29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="1"/>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="1"/>
-      <c r="D31" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="1"/>
-      <c r="D32" t="s">
-        <v>36</v>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="1"/>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="1"/>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="1"/>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="1">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
+      <c r="B37" s="1"/>
+      <c r="D37" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="1"/>
       <c r="D38" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="1"/>
-      <c r="D39" t="s">
-        <v>37</v>
-      </c>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="1"/>
-      <c r="D40" t="s">
-        <v>40</v>
+      <c r="B40" s="1">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="1"/>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="1"/>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="1"/>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="D44" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="1">
-        <v>6</v>
-      </c>
-      <c r="C45" t="s">
-        <v>13</v>
+      <c r="B45" s="1"/>
+      <c r="D45" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="1"/>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="1"/>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="1"/>
-      <c r="D48" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="1"/>
-      <c r="D49" t="s">
-        <v>45</v>
+      <c r="B49" s="1">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" s="1"/>
       <c r="D50" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" s="1"/>
       <c r="D51" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="1"/>
       <c r="D52" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="2:4">
-      <c r="B53" s="1"/>
+      <c r="D53" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="1">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
-        <v>14</v>
+      <c r="D54" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" s="1"/>
       <c r="D55" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="2:4">
-      <c r="B56" s="1"/>
       <c r="D56" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="B57" s="1"/>
-      <c r="D57" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="2:4">
-      <c r="D58" t="s">
-        <v>30</v>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="D59" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="D60" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="D61" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="D62" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="2:4">
-      <c r="B63">
-        <v>8</v>
-      </c>
-      <c r="C63" t="s">
-        <v>15</v>
+      <c r="D63" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="D64" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="D65" t="s">
-        <v>33</v>
-      </c>
+      <c r="D65" s="1"/>
     </row>
     <row r="66" spans="2:4">
-      <c r="D66" t="s">
-        <v>34</v>
+      <c r="B66">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="D67" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="2:4">
-      <c r="D68" t="s">
-        <v>39</v>
+      <c r="D68" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="D69" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="2:4">
-      <c r="D70" s="1"/>
+      <c r="D70" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="71" spans="2:4">
-      <c r="B71">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
-        <v>16</v>
+      <c r="D71" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="D72" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="2:4">
-      <c r="D73" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D73" s="1"/>
     </row>
     <row r="74" spans="2:4">
-      <c r="D74" t="s">
-        <v>36</v>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="D75" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="D76" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="D77" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="2:4">
-      <c r="D78" s="1"/>
+      <c r="D78" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="79" spans="2:4">
-      <c r="B79">
-        <v>10</v>
-      </c>
-      <c r="C79" t="s">
-        <v>18</v>
+      <c r="D79" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="D80" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="81" spans="2:4">
-      <c r="D81" t="s">
-        <v>37</v>
-      </c>
+      <c r="D81" s="1"/>
     </row>
     <row r="82" spans="2:4">
-      <c r="D82" t="s">
-        <v>40</v>
+      <c r="B82">
+        <v>11</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="D83" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="D84" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="D85" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="2:4">
-      <c r="D86" s="1"/>
+      <c r="D86" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="87" spans="2:4">
-      <c r="B87">
-        <v>11</v>
-      </c>
-      <c r="C87" t="s">
-        <v>19</v>
+      <c r="D87" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="D88" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="D89" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4">
-      <c r="D90" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="2:4">
-      <c r="D91" t="s">
-        <v>45</v>
+      <c r="B91">
+        <v>12</v>
+      </c>
+      <c r="C91" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="D92" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4">
-      <c r="D93" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="D95" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="D96" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4">
-      <c r="D94" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4">
-      <c r="B96">
-        <v>12</v>
-      </c>
-      <c r="C96" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="97" spans="2:4">
       <c r="D97" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="D100" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="D101" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4">
-      <c r="D102" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="C103" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="D104" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4">
-      <c r="B104">
-        <v>14</v>
-      </c>
-      <c r="C104" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="105" spans="2:4">
@@ -1472,71 +1509,48 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="2:4">
-      <c r="D106" t="s">
-        <v>51</v>
+    <row r="107" spans="2:4">
+      <c r="B107">
+        <v>16</v>
+      </c>
+      <c r="C107" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="2:4">
-      <c r="B108">
-        <v>15</v>
-      </c>
-      <c r="C108" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4">
-      <c r="D109" t="s">
-        <v>55</v>
+      <c r="D108" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="110" spans="2:4">
-      <c r="D110" t="s">
-        <v>56</v>
+      <c r="B110">
+        <v>17</v>
+      </c>
+      <c r="C110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="D111" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="2:4">
-      <c r="B112">
-        <v>16</v>
-      </c>
-      <c r="C112" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4">
-      <c r="D113" t="s">
-        <v>52</v>
+      <c r="D112" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114">
+        <v>18</v>
+      </c>
+      <c r="C114" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="115" spans="2:4">
-      <c r="B115">
-        <v>17</v>
-      </c>
-      <c r="C115" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4">
-      <c r="D116" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="D117" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4">
-      <c r="B119">
-        <v>18</v>
-      </c>
-      <c r="C119" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4">
-      <c r="D120" t="s">
-        <v>174</v>
+      <c r="D115" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1547,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D78"/>
+  <dimension ref="B1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1558,318 +1572,410 @@
     <col min="3" max="3" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:5">
       <c r="B1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1"/>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1">
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="1"/>
-      <c r="D9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="D8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="E9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="D10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="D13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="D14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="D17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="D18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="D19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="D22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="E23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="D25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="D25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="D26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="D28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:5">
       <c r="D29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
-      <c r="D30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32">
-        <v>21</v>
-      </c>
-      <c r="C32" t="s">
-        <v>125</v>
+    <row r="31" spans="2:5">
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="D32" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="D33" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="D34" t="s">
-        <v>127</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36">
-        <v>22</v>
-      </c>
-      <c r="C36" t="s">
-        <v>124</v>
+      <c r="D36" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="D37" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="D38" t="s">
-        <v>128</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s">
-        <v>129</v>
+      <c r="D40" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="D41" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="D42" t="s">
-        <v>131</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44">
-        <v>24</v>
-      </c>
-      <c r="C44" t="s">
-        <v>132</v>
+      <c r="D44" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="D45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4">
-      <c r="D46" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="2:4">
-      <c r="D47" t="s">
-        <v>135</v>
+      <c r="B47">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="D48" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="D49" t="s">
-        <v>137</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="D50" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51">
-        <v>25</v>
-      </c>
-      <c r="C51" t="s">
-        <v>141</v>
+      <c r="D51" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="D52" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="D53" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="2:4">
-      <c r="D54" t="s">
-        <v>143</v>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="D55" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="2:4">
-      <c r="B56">
-        <v>26</v>
-      </c>
-      <c r="C56" t="s">
-        <v>145</v>
+      <c r="D56" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="D58" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="2:4">
-      <c r="D59" t="s">
-        <v>148</v>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="D60" t="s">
-        <v>149</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="D61" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62">
-        <v>24</v>
-      </c>
-      <c r="C62" t="s">
-        <v>150</v>
+      <c r="D62" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="D63" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4">
-      <c r="D64" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="D65" t="s">
-        <v>135</v>
+      <c r="B65">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="D66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="D67" t="s">
-        <v>137</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="D68" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="2:4">
-      <c r="B69">
-        <v>25</v>
-      </c>
-      <c r="C69" t="s">
-        <v>151</v>
+      <c r="D69" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="D70" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4">
-      <c r="D71" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="2:4">
-      <c r="D72" t="s">
-        <v>143</v>
+      <c r="B72">
+        <v>25</v>
+      </c>
+      <c r="C72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="D73" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="2:4">
-      <c r="B74">
-        <v>26</v>
-      </c>
-      <c r="C74" t="s">
-        <v>152</v>
+      <c r="D74" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="D75" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4">
-      <c r="D76" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="2:4">
-      <c r="D77" t="s">
-        <v>148</v>
+      <c r="B77">
+        <v>26</v>
+      </c>
+      <c r="C77" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="D78" t="s">
-        <v>149</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="D79" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="D80" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="D81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83">
+        <v>27</v>
+      </c>
+      <c r="C83" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="D84" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="D85" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="D86" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1879,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E142"/>
+  <dimension ref="B1:E138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1893,681 +1999,661 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1"/>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1"/>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1"/>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="D11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="1"/>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="1"/>
-      <c r="D10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="1"/>
-      <c r="E11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="D14" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="D15" t="s">
-        <v>118</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="D16" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>77</v>
+      <c r="D17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="D18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="D19" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="D20" t="s">
-        <v>80</v>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="D22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="D23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="D25" t="s">
-        <v>96</v>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="D26" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="D27" t="s">
-        <v>97</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="D28" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
+      <c r="D29" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="D30" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="D31" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="D32" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:4">
-      <c r="D33" t="s">
-        <v>87</v>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="D34" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="D35" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="D36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>88</v>
+      <c r="D37" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="D38" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="D39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="D40" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="D41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="D42" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="D43" t="s">
-        <v>41</v>
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="D44" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="D45" t="s">
-        <v>89</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="D46" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>91</v>
+      <c r="D47" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="D48" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="D49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="D50" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="D51" t="s">
-        <v>87</v>
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="D52" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="D53" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>175</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="D54" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="2:4">
-      <c r="D56" t="s">
-        <v>176</v>
+      <c r="B56">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" t="s">
-        <v>177</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="D58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4">
-      <c r="B60">
-        <v>9</v>
-      </c>
-      <c r="C60" t="s">
-        <v>92</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="D59" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="D61" t="s">
-        <v>93</v>
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="D62" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="D63" t="s">
-        <v>95</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="D64" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="B65">
-        <v>10</v>
-      </c>
-      <c r="C65" t="s">
-        <v>98</v>
+      <c r="D65" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="D66" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="D67" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="D68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4">
-      <c r="D69" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="2:4">
-      <c r="D70" t="s">
-        <v>39</v>
+      <c r="B70">
+        <v>11</v>
+      </c>
+      <c r="C70" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="D71" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="D72" t="s">
-        <v>119</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="D73" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="2:4">
-      <c r="B74">
-        <v>11</v>
-      </c>
-      <c r="C74" t="s">
-        <v>99</v>
+      <c r="D74" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="D75" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="D76" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="D77" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="D78" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="D79" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4">
-      <c r="D80" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="2:4">
-      <c r="D81" t="s">
-        <v>90</v>
+      <c r="B81">
+        <v>12</v>
+      </c>
+      <c r="C81" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="D82" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="D83" t="s">
-        <v>119</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="D84" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85">
-        <v>12</v>
-      </c>
-      <c r="C85" t="s">
-        <v>100</v>
+      <c r="D85" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="D86" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="2:4">
       <c r="D87" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="D88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4">
-      <c r="D89" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="2:4">
-      <c r="D90" t="s">
-        <v>39</v>
+      <c r="B90">
+        <v>13</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="D91" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="D92" t="s">
-        <v>119</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="D93" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94">
-        <v>13</v>
-      </c>
-      <c r="C94" t="s">
-        <v>120</v>
+      <c r="D94" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="D95" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="D96" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="2:4">
       <c r="D97" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4">
-      <c r="D98" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="2:4">
-      <c r="D99" t="s">
-        <v>39</v>
+      <c r="B99">
+        <v>14</v>
+      </c>
+      <c r="C99" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="D100" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="D101" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="B103">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="D104" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="2:4">
       <c r="D105" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="2:4">
       <c r="B107">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="D108" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="2:4">
       <c r="D109" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="111" spans="2:4">
       <c r="B111">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C111" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="D112" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="2:4">
       <c r="D113" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="B115">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C115" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="D116" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="D117" t="s">
-        <v>114</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="B118">
+        <v>19</v>
+      </c>
+      <c r="C118" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="2:4">
-      <c r="B119">
-        <v>18</v>
-      </c>
-      <c r="C119" t="s">
-        <v>116</v>
+      <c r="D119" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="D120" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="2:4">
       <c r="B122">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C122" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="123" spans="2:4">
       <c r="D123" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="124" spans="2:4">
-      <c r="D124" t="s">
-        <v>158</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4">
+      <c r="B125">
+        <v>21</v>
+      </c>
+      <c r="C125" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="126" spans="2:4">
-      <c r="B126">
-        <v>20</v>
-      </c>
-      <c r="C126" t="s">
-        <v>159</v>
+      <c r="D126" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="127" spans="2:4">
       <c r="D127" t="s">
-        <v>160</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4">
+      <c r="D128" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="2:4">
-      <c r="B129">
-        <v>21</v>
-      </c>
-      <c r="C129" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4">
-      <c r="D130" t="s">
-        <v>162</v>
+      <c r="D129" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="2:4">
-      <c r="D131" t="s">
-        <v>163</v>
+      <c r="B131">
+        <v>22</v>
+      </c>
+      <c r="C131" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="132" spans="2:4">
       <c r="D132" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="133" spans="2:4">
-      <c r="D133" t="s">
-        <v>165</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4">
+      <c r="B134">
+        <v>23</v>
+      </c>
+      <c r="C134" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="135" spans="2:4">
-      <c r="B135">
-        <v>22</v>
-      </c>
-      <c r="C135" t="s">
-        <v>166</v>
+      <c r="D135" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="136" spans="2:4">
       <c r="D136" t="s">
-        <v>167</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4">
+      <c r="D137" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="138" spans="2:4">
-      <c r="B138">
-        <v>23</v>
-      </c>
-      <c r="C138" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="139" spans="2:4">
-      <c r="D139" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="140" spans="2:4">
-      <c r="D140" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="141" spans="2:4">
-      <c r="D141" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="142" spans="2:4">
-      <c r="D142" t="s">
-        <v>172</v>
+      <c r="D138" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2578,27 +2664,91 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:B3"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:4">
       <c r="B1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1"/>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="D8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="D12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="D14" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>